<commit_message>
deixando o vendedor ser um campo opcional
</commit_message>
<xml_diff>
--- a/projeto/backend/arquivos_mock/Vendas.xlsx
+++ b/projeto/backend/arquivos_mock/Vendas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14" count="14">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10" count="10">
   <x:si>
     <x:t>data</x:t>
   </x:si>
@@ -56,6 +56,9 @@
   </x:si>
   <x:si>
     <x:t>Adjamir de Moura Galvão</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22/02/2023</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -503,6 +506,23 @@
         <x:v>2</x:v>
       </x:c>
     </x:row>
+    <x:row r="6" spans="1:5">
+      <x:c r="A6" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="n">
+        <x:v>-108.01</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>